<commit_message>
fixeda typo in a label of the public event types controlled vocabulary
</commit_message>
<xml_diff>
--- a/VocabolariControllati/public-event-types/public-event-types.xlsx
+++ b/VocabolariControllati/public-event-types/public-event-types.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/EventiPubblici/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/public-event-types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE131BC1-6427-DA49-8E33-8D097DBEC07C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAA474C-4D8D-0245-96D9-EF362111081C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{428B79BD-67F6-484C-96F4-F73B1CE52F32}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Terzo livello" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -982,9 +981,6 @@
   </si>
   <si>
     <t>Sport show</t>
-  </si>
-  <si>
-    <t>Maniferstazioni sportive</t>
   </si>
   <si>
     <t>Sport shows</t>
@@ -1181,6 +1177,9 @@
   </si>
   <si>
     <t>Political procession / strike</t>
+  </si>
+  <si>
+    <t>Manifestazioni sportive</t>
   </si>
 </sst>
 </file>
@@ -1619,8 +1618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21961AD0-8627-8E4C-A7C3-A119FB0EA6A3}">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N51" zoomScale="149" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+    <sheetView tabSelected="1" topLeftCell="H52" zoomScale="149" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1744,7 +1743,7 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>22</v>
@@ -1794,7 +1793,7 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>22</v>
@@ -1846,7 +1845,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>22</v>
@@ -1906,7 +1905,7 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>22</v>
@@ -1966,7 +1965,7 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>22</v>
@@ -2026,7 +2025,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>22</v>
@@ -2080,7 +2079,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>22</v>
@@ -2134,7 +2133,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>22</v>
@@ -2146,7 +2145,7 @@
         <v>53</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>54</v>
@@ -2194,7 +2193,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>22</v>
@@ -2250,7 +2249,7 @@
         <v>206</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>64</v>
@@ -2259,10 +2258,10 @@
         <v>65</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>67</v>
@@ -2306,7 +2305,7 @@
         <v>206</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>64</v>
@@ -2360,7 +2359,7 @@
         <v>206</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>64</v>
@@ -2416,7 +2415,7 @@
         <v>206</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>64</v>
@@ -2472,7 +2471,7 @@
         <v>206</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>64</v>
@@ -2487,7 +2486,7 @@
         <v>81</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -2528,7 +2527,7 @@
         <v>206</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>64</v>
@@ -2588,7 +2587,7 @@
         <v>205</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>124</v>
@@ -2597,7 +2596,7 @@
         <v>121</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>79</v>
@@ -2606,7 +2605,7 @@
         <v>126</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -2646,7 +2645,7 @@
         <v>205</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>124</v>
@@ -2661,10 +2660,10 @@
         <v>129</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="208">
@@ -2702,7 +2701,7 @@
         <v>205</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>124</v>
@@ -2751,7 +2750,7 @@
         <v>148</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>149</v>
@@ -2769,7 +2768,7 @@
         <v>98</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>139</v>
@@ -2786,7 +2785,7 @@
         <v>93</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>140</v>
@@ -2831,7 +2830,7 @@
         <v>153</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>160</v>
@@ -2848,7 +2847,7 @@
         <v>93</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>140</v>
@@ -2904,7 +2903,7 @@
         <v>93</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>140</v>
@@ -2940,13 +2939,13 @@
         <v>168</v>
       </c>
       <c r="O23" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="Q23" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>170</v>
@@ -2960,7 +2959,7 @@
         <v>93</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>140</v>
@@ -3010,7 +3009,7 @@
         <v>93</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>140</v>
@@ -3046,7 +3045,7 @@
         <v>178</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>181</v>
@@ -3066,7 +3065,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>140</v>
@@ -3102,7 +3101,7 @@
         <v>183</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>184</v>
@@ -3116,7 +3115,7 @@
         <v>93</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>140</v>
@@ -3140,7 +3139,7 @@
         <v>106</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>188</v>
@@ -3158,10 +3157,10 @@
         <v>197</v>
       </c>
       <c r="S27" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="T27" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="144">
@@ -3172,7 +3171,7 @@
         <v>93</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>140</v>
@@ -3196,7 +3195,7 @@
         <v>106</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>188</v>
@@ -3225,7 +3224,7 @@
         <v>93</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>140</v>
@@ -3249,7 +3248,7 @@
         <v>106</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>188</v>
@@ -3275,7 +3274,7 @@
         <v>93</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>140</v>
@@ -3299,7 +3298,7 @@
         <v>106</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>188</v>
@@ -3308,13 +3307,13 @@
         <v>192</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="144">
@@ -3325,7 +3324,7 @@
         <v>93</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>140</v>
@@ -3349,7 +3348,7 @@
         <v>106</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>188</v>
@@ -3375,7 +3374,7 @@
         <v>93</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>140</v>
@@ -3399,7 +3398,7 @@
         <v>106</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>188</v>
@@ -3425,7 +3424,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>140</v>
@@ -3450,7 +3449,7 @@
       </c>
       <c r="K33" s="10"/>
       <c r="L33" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>219</v>
@@ -3476,7 +3475,7 @@
         <v>93</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>140</v>
@@ -3501,7 +3500,7 @@
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>219</v>
@@ -3527,7 +3526,7 @@
         <v>93</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>140</v>
@@ -3552,7 +3551,7 @@
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>219</v>
@@ -3578,7 +3577,7 @@
         <v>93</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>140</v>
@@ -3603,7 +3602,7 @@
       </c>
       <c r="K36" s="10"/>
       <c r="L36" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>219</v>
@@ -3629,7 +3628,7 @@
         <v>93</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>140</v>
@@ -3654,7 +3653,7 @@
       </c>
       <c r="K37" s="10"/>
       <c r="L37" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>219</v>
@@ -3680,7 +3679,7 @@
         <v>93</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>140</v>
@@ -3705,7 +3704,7 @@
       </c>
       <c r="K38" s="10"/>
       <c r="L38" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>219</v>
@@ -3723,10 +3722,10 @@
         <v>231</v>
       </c>
       <c r="S38" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="T38" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="T38" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="80">
@@ -3737,7 +3736,7 @@
         <v>93</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>140</v>
@@ -3762,7 +3761,7 @@
       </c>
       <c r="K39" s="10"/>
       <c r="L39" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>219</v>
@@ -3815,7 +3814,7 @@
         <v>256</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>257</v>
@@ -3880,7 +3879,7 @@
         <v>263</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>264</v>
@@ -3974,7 +3973,7 @@
         <v>274</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>275</v>
@@ -4283,34 +4282,34 @@
         <v>114</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>315</v>
       </c>
       <c r="J49" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K49" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="L49" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M49" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>307</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="64">
@@ -4342,28 +4341,28 @@
         <v>315</v>
       </c>
       <c r="J50" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M50" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>312</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="64">
@@ -4395,28 +4394,28 @@
         <v>315</v>
       </c>
       <c r="J51" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="L51" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M51" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>313</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="64">
@@ -4448,28 +4447,28 @@
         <v>315</v>
       </c>
       <c r="J52" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K52" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="L52" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M52" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="L52" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="N52" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="64">
@@ -4501,28 +4500,28 @@
         <v>315</v>
       </c>
       <c r="J53" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K53" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="L53" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M53" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="L53" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="N53" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="64">
@@ -4554,28 +4553,28 @@
         <v>315</v>
       </c>
       <c r="J54" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K54" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="L54" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M54" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="L54" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="N54" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -5281,7 +5280,7 @@
         <v>307</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5289,7 +5288,7 @@
         <v>312</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5297,31 +5296,31 @@
         <v>313</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>